<commit_message>
still dealing with the prod error
</commit_message>
<xml_diff>
--- a/hoja_de_vida/hdv_temp.xlsx
+++ b/hoja_de_vida/hdv_temp.xlsx
@@ -1307,7 +1307,7 @@
       <c r="B6" s="114" t="n"/>
       <c r="C6" s="90" t="inlineStr">
         <is>
-          <t>sdsds</t>
+          <t>fggfelñ</t>
         </is>
       </c>
       <c r="D6" s="111" t="n"/>
@@ -1326,7 +1326,7 @@
       <c r="B7" s="114" t="n"/>
       <c r="C7" s="90" t="inlineStr">
         <is>
-          <t>xxzvxv</t>
+          <t>efgego</t>
         </is>
       </c>
       <c r="D7" s="111" t="n"/>
@@ -1345,7 +1345,7 @@
       <c r="B8" s="114" t="n"/>
       <c r="C8" s="90" t="inlineStr">
         <is>
-          <t>sdds</t>
+          <t>wdfedop</t>
         </is>
       </c>
       <c r="D8" s="111" t="n"/>
@@ -1364,7 +1364,7 @@
       <c r="B9" s="114" t="n"/>
       <c r="C9" s="92" t="inlineStr">
         <is>
-          <t>sdfsd</t>
+          <t>deop</t>
         </is>
       </c>
       <c r="D9" s="111" t="n"/>
@@ -1383,7 +1383,7 @@
       <c r="B10" s="114" t="n"/>
       <c r="C10" s="93" t="inlineStr">
         <is>
-          <t>sdsdf</t>
+          <t>ege</t>
         </is>
       </c>
       <c r="D10" s="111" t="n"/>
@@ -1402,7 +1402,7 @@
       <c r="B11" s="114" t="n"/>
       <c r="C11" s="96" t="inlineStr">
         <is>
-          <t>assdf</t>
+          <t>wfeg</t>
         </is>
       </c>
       <c r="D11" s="111" t="n"/>

</xml_diff>